<commit_message>
JPY Libor calendar workaround
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/JPY_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/JPY_MainChecks.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15285" yWindow="-15" windowWidth="15330" windowHeight="8205"/>
+    <workbookView xWindow="7515" yWindow="-15" windowWidth="7530" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Currency">MainChecks!$B$1</definedName>
     <definedName name="EvaluationDate">MainChecks!$C$5</definedName>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ObjectID</t>
   </si>
@@ -57,6 +60,9 @@
   <si>
     <t>JpyLibor6M</t>
   </si>
+  <si>
+    <t>MarketUpdates</t>
+  </si>
 </sst>
 </file>
 
@@ -64,14 +70,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="9">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="ddd\,\ dd\-mmm\-yyyy"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0;#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="General_)"/>
-    <numFmt numFmtId="170" formatCode="ddd\,\ dd\-mmm\-yyyy\,\ hh:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="ddd\,\ d\-mmm\-yyyy"/>
-    <numFmt numFmtId="172" formatCode="yyyy\-mmm\-dd\-hh:mm:ss"/>
-    <numFmt numFmtId="174" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="ddd\,\ dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0;#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="General_)"/>
+    <numFmt numFmtId="169" formatCode="ddd\,\ dd\-mmm\-yyyy\,\ hh:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="171" formatCode="yyyy\-mmm\-dd\-hh:mm:ss"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -141,7 +147,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +184,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -438,13 +450,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -453,60 +495,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -522,15 +510,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="0">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -548,7 +536,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="170" fontId="8" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -558,7 +546,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,73 +553,84 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="6" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="11" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="172" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="170" fontId="6" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -727,9 +725,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:17:38</v>
+        <v>Updated at 16:37:30</v>
         <stp/>
-        <stp>{3D81532D-E45D-45B6-BB11-D8C779F687ED}</stp>
+        <stp>{92D505DB-27C5-444C-87A6-1B49FE8D20AF}</stp>
         <tr r="I4" s="2"/>
       </tp>
     </main>
@@ -830,6 +828,170 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="General Settings"/>
+      <sheetName val="Libor"/>
+      <sheetName val="Tibor"/>
+      <sheetName val="LiborSwapIsdaFixAm"/>
+      <sheetName val="LiborSwapForBasisCalc"/>
+      <sheetName val="LiborSwapIsdaFixPm"/>
+      <sheetName val="Deposits"/>
+      <sheetName val="OIS"/>
+      <sheetName val="FRA"/>
+      <sheetName val="Futures3M_TIBOR"/>
+      <sheetName val="Futures3M"/>
+      <sheetName val="FuturesHWConvAdj"/>
+      <sheetName val="BasisSwap1MxM"/>
+      <sheetName val="BasisSwap3M6M"/>
+      <sheetName val="Swap3M_TIBOR"/>
+      <sheetName val="Swap6M"/>
+      <sheetName val="Swaps1M"/>
+      <sheetName val="Swap3M"/>
+      <sheetName val="ON"/>
+      <sheetName val="1M (2)"/>
+      <sheetName val="3M (2)"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="D7">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="7">
+          <cell r="D7">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6M</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>Fwd Curve</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6M</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>JPYSND_Quote#0000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>3W</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>JPY3x6F_Quote</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>N4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>N4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="13">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="14">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>3T</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="15">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="16">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>X1S</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="17">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>3L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="20">
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>6L</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,7 +1284,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W101"/>
+  <dimension ref="A1:W102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -1130,16 +1292,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="6" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -1172,24 +1334,24 @@
     </row>
     <row r="2" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="31" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="24"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="10"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1207,23 +1369,25 @@
     </row>
     <row r="3" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="29">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote")</f>
-        <v>41828</v>
+      <c r="C3" s="40">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41820</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="30">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote")</f>
-        <v>1.7857000000000001E-3</v>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42" t="e">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NUM!</v>
       </c>
-      <c r="F3" s="31" t="str">
-        <f>IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v/>
+      <c r="F3" s="43" t="str">
+        <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
+        <v>qlQuoteValue - 1st iteration: failed at 27th alive instrument, maturity May 27th, 2044, reference date May 27th, 2014: 1st leg: time (30.0356) is past max curve time (30.0329)</v>
       </c>
       <c r="G3" s="8"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="10"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -1241,18 +1405,18 @@
     </row>
     <row r="4" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41" t="str">
+      <c r="I4" s="48" t="str">
         <f>_xll.RData(H5,"LAST",,"FRQ:1S",,I5)</f>
-        <v>Updated at 11:17:38</v>
+        <v>Updated at 16:37:30</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="5"/>
@@ -1269,18 +1433,18 @@
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="42" t="str">
+      <c r="B5" s="33" t="str">
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>JPYSTD</v>
       </c>
-      <c r="C5" s="43">
-        <f>_xll.qlTermStructureReferenceDate(B5)</f>
-        <v>41829</v>
+      <c r="C5" s="34">
+        <f>_xll.qlTermStructureReferenceDate(B5,Trigger)</f>
+        <v>41781</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45">
+      <c r="D5" s="35"/>
+      <c r="E5" s="36">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
         <v>1</v>
       </c>
@@ -1289,11 +1453,11 @@
         <v/>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="25">
-        <v>147.36000000000001</v>
+      <c r="I5" s="50">
+        <v>147.38</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="5"/>
@@ -1316,12 +1480,12 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>JPYON</v>
       </c>
-      <c r="C6" s="34">
-        <f>_xll.qlTermStructureReferenceDate(B6)</f>
-        <v>41829</v>
+      <c r="C6" s="26">
+        <f>_xll.qlTermStructureReferenceDate(B6,Trigger)</f>
+        <v>41781</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="46">
+      <c r="E6" s="37">
         <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
         <v>1</v>
       </c>
@@ -1330,6 +1494,13 @@
         <v/>
       </c>
       <c r="G6" s="8"/>
+      <c r="H6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="52">
+        <f>[1]!TriggerCounter</f>
+        <v>2</v>
+      </c>
       <c r="J6" s="10"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1345,33 +1516,28 @@
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="12" t="str">
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>JPY3M</v>
       </c>
-      <c r="C7" s="34">
-        <f>_xll.qlTermStructureReferenceDate(B7)</f>
-        <v>41831</v>
+      <c r="C7" s="26">
+        <f>_xll.qlTermStructureReferenceDate(B7,Trigger)</f>
+        <v>41786</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="E7" s="46">
+      <c r="E7" s="37" t="e">
         <f>_xll.qlYieldTSDiscount(B7,C7,,Trigger)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="F7" s="14" t="str">
-        <f>IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
+        <v>qlYieldTSDiscount - 1st iteration: failed at 24th alive instrument, maturity May 27th, 2044, reference date May 27th, 2014: 1st leg: time (30.0356) is past max curve time (30.0329)</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="16">
-        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1229</v>
-      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="10"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1389,30 +1555,30 @@
     </row>
     <row r="8" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="32" t="str">
+      <c r="B8" s="24" t="str">
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>JPY6M</v>
       </c>
-      <c r="C8" s="35">
-        <f>_xll.qlTermStructureReferenceDate(B8)</f>
-        <v>41831</v>
+      <c r="C8" s="27">
+        <f>_xll.qlTermStructureReferenceDate(B8,Trigger)</f>
+        <v>41786</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="47">
+      <c r="D8" s="25"/>
+      <c r="E8" s="38" t="e">
         <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
-      <c r="F8" s="18" t="str">
-        <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v/>
+      <c r="F8" s="17" t="str">
+        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
+        <v>qlYieldTSDiscount - 1st iteration: failed at 27th alive instrument, maturity May 27th, 2044, reference date May 27th, 2014: 1st leg: time (30.0356) is past max curve time (30.0329)</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="19" t="s">
-        <v>9</v>
+      <c r="H8" s="15" t="s">
+        <v>4</v>
       </c>
-      <c r="I8" s="20" t="str">
-        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_52 / 1.5.0 / 1.5</v>
+      <c r="I8" s="16">
+        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
+        <v>1158</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="5"/>
@@ -1430,16 +1596,21 @@
       <c r="W8" s="5"/>
     </row>
     <row r="9" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="19" t="str">
+        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
+        <v>1_52 / 1.5.0 / 1.5</v>
+      </c>
+      <c r="J9" s="10"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -1454,17 +1625,17 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+    <row r="10" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -2461,10 +2632,10 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
@@ -2480,16 +2651,16 @@
       <c r="W50" s="5"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
@@ -2505,16 +2676,16 @@
       <c r="W51" s="5"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
@@ -2530,16 +2701,16 @@
       <c r="W52" s="5"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
@@ -2555,1174 +2726,1199 @@
       <c r="W53" s="5"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="27"/>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="27"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="27"/>
-      <c r="T54" s="27"/>
-      <c r="U54" s="27"/>
-      <c r="V54" s="27"/>
-      <c r="W54" s="27"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="27"/>
-      <c r="L55" s="27"/>
-      <c r="M55" s="27"/>
-      <c r="N55" s="27"/>
-      <c r="O55" s="27"/>
-      <c r="P55" s="27"/>
-      <c r="Q55" s="27"/>
-      <c r="R55" s="27"/>
-      <c r="S55" s="27"/>
-      <c r="T55" s="27"/>
-      <c r="U55" s="27"/>
-      <c r="V55" s="27"/>
-      <c r="W55" s="27"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="23"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="23"/>
+      <c r="S55" s="23"/>
+      <c r="T55" s="23"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="23"/>
+      <c r="W55" s="23"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="27"/>
-      <c r="T56" s="27"/>
-      <c r="U56" s="27"/>
-      <c r="V56" s="27"/>
-      <c r="W56" s="27"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23"/>
+      <c r="P56" s="23"/>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="23"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="23"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="23"/>
+      <c r="W56" s="23"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="27"/>
-      <c r="L57" s="27"/>
-      <c r="M57" s="27"/>
-      <c r="N57" s="27"/>
-      <c r="O57" s="27"/>
-      <c r="P57" s="27"/>
-      <c r="Q57" s="27"/>
-      <c r="R57" s="27"/>
-      <c r="S57" s="27"/>
-      <c r="T57" s="27"/>
-      <c r="U57" s="27"/>
-      <c r="V57" s="27"/>
-      <c r="W57" s="27"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="23"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="23"/>
+      <c r="S57" s="23"/>
+      <c r="T57" s="23"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="23"/>
+      <c r="W57" s="23"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="27"/>
-      <c r="N58" s="27"/>
-      <c r="O58" s="27"/>
-      <c r="P58" s="27"/>
-      <c r="Q58" s="27"/>
-      <c r="R58" s="27"/>
-      <c r="S58" s="27"/>
-      <c r="T58" s="27"/>
-      <c r="U58" s="27"/>
-      <c r="V58" s="27"/>
-      <c r="W58" s="27"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23"/>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="23"/>
+      <c r="S58" s="23"/>
+      <c r="T58" s="23"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="23"/>
+      <c r="W58" s="23"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="27"/>
-      <c r="L59" s="27"/>
-      <c r="M59" s="27"/>
-      <c r="N59" s="27"/>
-      <c r="O59" s="27"/>
-      <c r="P59" s="27"/>
-      <c r="Q59" s="27"/>
-      <c r="R59" s="27"/>
-      <c r="S59" s="27"/>
-      <c r="T59" s="27"/>
-      <c r="U59" s="27"/>
-      <c r="V59" s="27"/>
-      <c r="W59" s="27"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="23"/>
+      <c r="P59" s="23"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="23"/>
+      <c r="S59" s="23"/>
+      <c r="T59" s="23"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="23"/>
+      <c r="W59" s="23"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="27"/>
-      <c r="M60" s="27"/>
-      <c r="N60" s="27"/>
-      <c r="O60" s="27"/>
-      <c r="P60" s="27"/>
-      <c r="Q60" s="27"/>
-      <c r="R60" s="27"/>
-      <c r="S60" s="27"/>
-      <c r="T60" s="27"/>
-      <c r="U60" s="27"/>
-      <c r="V60" s="27"/>
-      <c r="W60" s="27"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
+      <c r="P60" s="23"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="23"/>
+      <c r="S60" s="23"/>
+      <c r="T60" s="23"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="23"/>
+      <c r="W60" s="23"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="27"/>
-      <c r="L61" s="27"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="27"/>
-      <c r="O61" s="27"/>
-      <c r="P61" s="27"/>
-      <c r="Q61" s="27"/>
-      <c r="R61" s="27"/>
-      <c r="S61" s="27"/>
-      <c r="T61" s="27"/>
-      <c r="U61" s="27"/>
-      <c r="V61" s="27"/>
-      <c r="W61" s="27"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="23"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="23"/>
+      <c r="S61" s="23"/>
+      <c r="T61" s="23"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="23"/>
+      <c r="W61" s="23"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="27"/>
-      <c r="N62" s="27"/>
-      <c r="O62" s="27"/>
-      <c r="P62" s="27"/>
-      <c r="Q62" s="27"/>
-      <c r="R62" s="27"/>
-      <c r="S62" s="27"/>
-      <c r="T62" s="27"/>
-      <c r="U62" s="27"/>
-      <c r="V62" s="27"/>
-      <c r="W62" s="27"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="23"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="23"/>
+      <c r="S62" s="23"/>
+      <c r="T62" s="23"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="23"/>
+      <c r="W62" s="23"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
-      <c r="J63" s="27"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="27"/>
-      <c r="M63" s="27"/>
-      <c r="N63" s="27"/>
-      <c r="O63" s="27"/>
-      <c r="P63" s="27"/>
-      <c r="Q63" s="27"/>
-      <c r="R63" s="27"/>
-      <c r="S63" s="27"/>
-      <c r="T63" s="27"/>
-      <c r="U63" s="27"/>
-      <c r="V63" s="27"/>
-      <c r="W63" s="27"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="23"/>
+      <c r="S63" s="23"/>
+      <c r="T63" s="23"/>
+      <c r="U63" s="23"/>
+      <c r="V63" s="23"/>
+      <c r="W63" s="23"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
-      <c r="N64" s="27"/>
-      <c r="O64" s="27"/>
-      <c r="P64" s="27"/>
-      <c r="Q64" s="27"/>
-      <c r="R64" s="27"/>
-      <c r="S64" s="27"/>
-      <c r="T64" s="27"/>
-      <c r="U64" s="27"/>
-      <c r="V64" s="27"/>
-      <c r="W64" s="27"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="23"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="23"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="23"/>
+      <c r="R64" s="23"/>
+      <c r="S64" s="23"/>
+      <c r="T64" s="23"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="23"/>
+      <c r="W64" s="23"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A65" s="27"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="N65" s="27"/>
-      <c r="O65" s="27"/>
-      <c r="P65" s="27"/>
-      <c r="Q65" s="27"/>
-      <c r="R65" s="27"/>
-      <c r="S65" s="27"/>
-      <c r="T65" s="27"/>
-      <c r="U65" s="27"/>
-      <c r="V65" s="27"/>
-      <c r="W65" s="27"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="23"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="23"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="23"/>
+      <c r="S65" s="23"/>
+      <c r="T65" s="23"/>
+      <c r="U65" s="23"/>
+      <c r="V65" s="23"/>
+      <c r="W65" s="23"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A66" s="27"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="27"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
-      <c r="N66" s="27"/>
-      <c r="O66" s="27"/>
-      <c r="P66" s="27"/>
-      <c r="Q66" s="27"/>
-      <c r="R66" s="27"/>
-      <c r="S66" s="27"/>
-      <c r="T66" s="27"/>
-      <c r="U66" s="27"/>
-      <c r="V66" s="27"/>
-      <c r="W66" s="27"/>
+      <c r="A66" s="23"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="23"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23"/>
+      <c r="S66" s="23"/>
+      <c r="T66" s="23"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="23"/>
+      <c r="W66" s="23"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="27"/>
-      <c r="P67" s="27"/>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27"/>
-      <c r="S67" s="27"/>
-      <c r="T67" s="27"/>
-      <c r="U67" s="27"/>
-      <c r="V67" s="27"/>
-      <c r="W67" s="27"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="23"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="23"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="23"/>
+      <c r="S67" s="23"/>
+      <c r="T67" s="23"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="23"/>
+      <c r="W67" s="23"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A68" s="27"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
-      <c r="I68" s="27"/>
-      <c r="J68" s="27"/>
-      <c r="K68" s="27"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="27"/>
-      <c r="O68" s="27"/>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="27"/>
-      <c r="S68" s="27"/>
-      <c r="T68" s="27"/>
-      <c r="U68" s="27"/>
-      <c r="V68" s="27"/>
-      <c r="W68" s="27"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="23"/>
+      <c r="N68" s="23"/>
+      <c r="O68" s="23"/>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="23"/>
+      <c r="S68" s="23"/>
+      <c r="T68" s="23"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="23"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A69" s="27"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="27"/>
-      <c r="M69" s="27"/>
-      <c r="N69" s="27"/>
-      <c r="O69" s="27"/>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="27"/>
-      <c r="S69" s="27"/>
-      <c r="T69" s="27"/>
-      <c r="U69" s="27"/>
-      <c r="V69" s="27"/>
-      <c r="W69" s="27"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="M69" s="23"/>
+      <c r="N69" s="23"/>
+      <c r="O69" s="23"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="23"/>
+      <c r="R69" s="23"/>
+      <c r="S69" s="23"/>
+      <c r="T69" s="23"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="23"/>
+      <c r="W69" s="23"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A70" s="27"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
-      <c r="J70" s="27"/>
-      <c r="K70" s="27"/>
-      <c r="L70" s="27"/>
-      <c r="M70" s="27"/>
-      <c r="N70" s="27"/>
-      <c r="O70" s="27"/>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="27"/>
-      <c r="R70" s="27"/>
-      <c r="S70" s="27"/>
-      <c r="T70" s="27"/>
-      <c r="U70" s="27"/>
-      <c r="V70" s="27"/>
-      <c r="W70" s="27"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="M70" s="23"/>
+      <c r="N70" s="23"/>
+      <c r="O70" s="23"/>
+      <c r="P70" s="23"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="23"/>
+      <c r="S70" s="23"/>
+      <c r="T70" s="23"/>
+      <c r="U70" s="23"/>
+      <c r="V70" s="23"/>
+      <c r="W70" s="23"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A71" s="27"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="27"/>
-      <c r="K71" s="27"/>
-      <c r="L71" s="27"/>
-      <c r="M71" s="27"/>
-      <c r="N71" s="27"/>
-      <c r="O71" s="27"/>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="27"/>
-      <c r="R71" s="27"/>
-      <c r="S71" s="27"/>
-      <c r="T71" s="27"/>
-      <c r="U71" s="27"/>
-      <c r="V71" s="27"/>
-      <c r="W71" s="27"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="23"/>
+      <c r="N71" s="23"/>
+      <c r="O71" s="23"/>
+      <c r="P71" s="23"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="23"/>
+      <c r="S71" s="23"/>
+      <c r="T71" s="23"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="23"/>
+      <c r="W71" s="23"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="27"/>
-      <c r="M72" s="27"/>
-      <c r="N72" s="27"/>
-      <c r="O72" s="27"/>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="27"/>
-      <c r="R72" s="27"/>
-      <c r="S72" s="27"/>
-      <c r="T72" s="27"/>
-      <c r="U72" s="27"/>
-      <c r="V72" s="27"/>
-      <c r="W72" s="27"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="23"/>
+      <c r="K72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="23"/>
+      <c r="O72" s="23"/>
+      <c r="P72" s="23"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="23"/>
+      <c r="S72" s="23"/>
+      <c r="T72" s="23"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="23"/>
+      <c r="W72" s="23"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A73" s="27"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="27"/>
-      <c r="K73" s="27"/>
-      <c r="L73" s="27"/>
-      <c r="M73" s="27"/>
-      <c r="N73" s="27"/>
-      <c r="O73" s="27"/>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="27"/>
-      <c r="R73" s="27"/>
-      <c r="S73" s="27"/>
-      <c r="T73" s="27"/>
-      <c r="U73" s="27"/>
-      <c r="V73" s="27"/>
-      <c r="W73" s="27"/>
+      <c r="A73" s="23"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
+      <c r="P73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="23"/>
+      <c r="S73" s="23"/>
+      <c r="T73" s="23"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="23"/>
+      <c r="W73" s="23"/>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A74" s="27"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
-      <c r="J74" s="27"/>
-      <c r="K74" s="27"/>
-      <c r="L74" s="27"/>
-      <c r="M74" s="27"/>
-      <c r="N74" s="27"/>
-      <c r="O74" s="27"/>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="27"/>
-      <c r="R74" s="27"/>
-      <c r="S74" s="27"/>
-      <c r="T74" s="27"/>
-      <c r="U74" s="27"/>
-      <c r="V74" s="27"/>
-      <c r="W74" s="27"/>
+      <c r="A74" s="23"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="23"/>
+      <c r="K74" s="23"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="23"/>
+      <c r="N74" s="23"/>
+      <c r="O74" s="23"/>
+      <c r="P74" s="23"/>
+      <c r="Q74" s="23"/>
+      <c r="R74" s="23"/>
+      <c r="S74" s="23"/>
+      <c r="T74" s="23"/>
+      <c r="U74" s="23"/>
+      <c r="V74" s="23"/>
+      <c r="W74" s="23"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A75" s="27"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
-      <c r="J75" s="27"/>
-      <c r="K75" s="27"/>
-      <c r="L75" s="27"/>
-      <c r="M75" s="27"/>
-      <c r="N75" s="27"/>
-      <c r="O75" s="27"/>
-      <c r="P75" s="27"/>
-      <c r="Q75" s="27"/>
-      <c r="R75" s="27"/>
-      <c r="S75" s="27"/>
-      <c r="T75" s="27"/>
-      <c r="U75" s="27"/>
-      <c r="V75" s="27"/>
-      <c r="W75" s="27"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="23"/>
+      <c r="K75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="M75" s="23"/>
+      <c r="N75" s="23"/>
+      <c r="O75" s="23"/>
+      <c r="P75" s="23"/>
+      <c r="Q75" s="23"/>
+      <c r="R75" s="23"/>
+      <c r="S75" s="23"/>
+      <c r="T75" s="23"/>
+      <c r="U75" s="23"/>
+      <c r="V75" s="23"/>
+      <c r="W75" s="23"/>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A76" s="27"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
-      <c r="J76" s="27"/>
-      <c r="K76" s="27"/>
-      <c r="L76" s="27"/>
-      <c r="M76" s="27"/>
-      <c r="N76" s="27"/>
-      <c r="O76" s="27"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="27"/>
-      <c r="S76" s="27"/>
-      <c r="T76" s="27"/>
-      <c r="U76" s="27"/>
-      <c r="V76" s="27"/>
-      <c r="W76" s="27"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="23"/>
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
+      <c r="O76" s="23"/>
+      <c r="P76" s="23"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="23"/>
+      <c r="S76" s="23"/>
+      <c r="T76" s="23"/>
+      <c r="U76" s="23"/>
+      <c r="V76" s="23"/>
+      <c r="W76" s="23"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A77" s="27"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="27"/>
-      <c r="L77" s="27"/>
-      <c r="M77" s="27"/>
-      <c r="N77" s="27"/>
-      <c r="O77" s="27"/>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="27"/>
-      <c r="R77" s="27"/>
-      <c r="S77" s="27"/>
-      <c r="T77" s="27"/>
-      <c r="U77" s="27"/>
-      <c r="V77" s="27"/>
-      <c r="W77" s="27"/>
+      <c r="A77" s="23"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
+      <c r="K77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="23"/>
+      <c r="N77" s="23"/>
+      <c r="O77" s="23"/>
+      <c r="P77" s="23"/>
+      <c r="Q77" s="23"/>
+      <c r="R77" s="23"/>
+      <c r="S77" s="23"/>
+      <c r="T77" s="23"/>
+      <c r="U77" s="23"/>
+      <c r="V77" s="23"/>
+      <c r="W77" s="23"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A78" s="27"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
-      <c r="J78" s="27"/>
-      <c r="K78" s="27"/>
-      <c r="L78" s="27"/>
-      <c r="M78" s="27"/>
-      <c r="N78" s="27"/>
-      <c r="O78" s="27"/>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="27"/>
-      <c r="R78" s="27"/>
-      <c r="S78" s="27"/>
-      <c r="T78" s="27"/>
-      <c r="U78" s="27"/>
-      <c r="V78" s="27"/>
-      <c r="W78" s="27"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+      <c r="J78" s="23"/>
+      <c r="K78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="M78" s="23"/>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23"/>
+      <c r="P78" s="23"/>
+      <c r="Q78" s="23"/>
+      <c r="R78" s="23"/>
+      <c r="S78" s="23"/>
+      <c r="T78" s="23"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="23"/>
+      <c r="W78" s="23"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A79" s="27"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="27"/>
-      <c r="K79" s="27"/>
-      <c r="L79" s="27"/>
-      <c r="M79" s="27"/>
-      <c r="N79" s="27"/>
-      <c r="O79" s="27"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="27"/>
-      <c r="R79" s="27"/>
-      <c r="S79" s="27"/>
-      <c r="T79" s="27"/>
-      <c r="U79" s="27"/>
-      <c r="V79" s="27"/>
-      <c r="W79" s="27"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
+      <c r="K79" s="23"/>
+      <c r="L79" s="23"/>
+      <c r="M79" s="23"/>
+      <c r="N79" s="23"/>
+      <c r="O79" s="23"/>
+      <c r="P79" s="23"/>
+      <c r="Q79" s="23"/>
+      <c r="R79" s="23"/>
+      <c r="S79" s="23"/>
+      <c r="T79" s="23"/>
+      <c r="U79" s="23"/>
+      <c r="V79" s="23"/>
+      <c r="W79" s="23"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="27"/>
-      <c r="N80" s="27"/>
-      <c r="O80" s="27"/>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="27"/>
-      <c r="R80" s="27"/>
-      <c r="S80" s="27"/>
-      <c r="T80" s="27"/>
-      <c r="U80" s="27"/>
-      <c r="V80" s="27"/>
-      <c r="W80" s="27"/>
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+      <c r="K80" s="23"/>
+      <c r="L80" s="23"/>
+      <c r="M80" s="23"/>
+      <c r="N80" s="23"/>
+      <c r="O80" s="23"/>
+      <c r="P80" s="23"/>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="23"/>
+      <c r="S80" s="23"/>
+      <c r="T80" s="23"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="23"/>
+      <c r="W80" s="23"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
-      <c r="L81" s="27"/>
-      <c r="M81" s="27"/>
-      <c r="N81" s="27"/>
-      <c r="O81" s="27"/>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="27"/>
-      <c r="R81" s="27"/>
-      <c r="S81" s="27"/>
-      <c r="T81" s="27"/>
-      <c r="U81" s="27"/>
-      <c r="V81" s="27"/>
-      <c r="W81" s="27"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="23"/>
+      <c r="K81" s="23"/>
+      <c r="L81" s="23"/>
+      <c r="M81" s="23"/>
+      <c r="N81" s="23"/>
+      <c r="O81" s="23"/>
+      <c r="P81" s="23"/>
+      <c r="Q81" s="23"/>
+      <c r="R81" s="23"/>
+      <c r="S81" s="23"/>
+      <c r="T81" s="23"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="23"/>
+      <c r="W81" s="23"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
-      <c r="J82" s="27"/>
-      <c r="K82" s="27"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="27"/>
-      <c r="N82" s="27"/>
-      <c r="O82" s="27"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="27"/>
-      <c r="R82" s="27"/>
-      <c r="S82" s="27"/>
-      <c r="T82" s="27"/>
-      <c r="U82" s="27"/>
-      <c r="V82" s="27"/>
-      <c r="W82" s="27"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="23"/>
+      <c r="L82" s="23"/>
+      <c r="M82" s="23"/>
+      <c r="N82" s="23"/>
+      <c r="O82" s="23"/>
+      <c r="P82" s="23"/>
+      <c r="Q82" s="23"/>
+      <c r="R82" s="23"/>
+      <c r="S82" s="23"/>
+      <c r="T82" s="23"/>
+      <c r="U82" s="23"/>
+      <c r="V82" s="23"/>
+      <c r="W82" s="23"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
-      <c r="J83" s="27"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="27"/>
-      <c r="N83" s="27"/>
-      <c r="O83" s="27"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="27"/>
-      <c r="R83" s="27"/>
-      <c r="S83" s="27"/>
-      <c r="T83" s="27"/>
-      <c r="U83" s="27"/>
-      <c r="V83" s="27"/>
-      <c r="W83" s="27"/>
+      <c r="A83" s="23"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="23"/>
+      <c r="K83" s="23"/>
+      <c r="L83" s="23"/>
+      <c r="M83" s="23"/>
+      <c r="N83" s="23"/>
+      <c r="O83" s="23"/>
+      <c r="P83" s="23"/>
+      <c r="Q83" s="23"/>
+      <c r="R83" s="23"/>
+      <c r="S83" s="23"/>
+      <c r="T83" s="23"/>
+      <c r="U83" s="23"/>
+      <c r="V83" s="23"/>
+      <c r="W83" s="23"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
-      <c r="J84" s="27"/>
-      <c r="K84" s="27"/>
-      <c r="L84" s="27"/>
-      <c r="M84" s="27"/>
-      <c r="N84" s="27"/>
-      <c r="O84" s="27"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27"/>
-      <c r="R84" s="27"/>
-      <c r="S84" s="27"/>
-      <c r="T84" s="27"/>
-      <c r="U84" s="27"/>
-      <c r="V84" s="27"/>
-      <c r="W84" s="27"/>
+      <c r="A84" s="23"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
+      <c r="J84" s="23"/>
+      <c r="K84" s="23"/>
+      <c r="L84" s="23"/>
+      <c r="M84" s="23"/>
+      <c r="N84" s="23"/>
+      <c r="O84" s="23"/>
+      <c r="P84" s="23"/>
+      <c r="Q84" s="23"/>
+      <c r="R84" s="23"/>
+      <c r="S84" s="23"/>
+      <c r="T84" s="23"/>
+      <c r="U84" s="23"/>
+      <c r="V84" s="23"/>
+      <c r="W84" s="23"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
-      <c r="J85" s="27"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="27"/>
-      <c r="M85" s="27"/>
-      <c r="N85" s="27"/>
-      <c r="O85" s="27"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="27"/>
-      <c r="R85" s="27"/>
-      <c r="S85" s="27"/>
-      <c r="T85" s="27"/>
-      <c r="U85" s="27"/>
-      <c r="V85" s="27"/>
-      <c r="W85" s="27"/>
+      <c r="A85" s="23"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="23"/>
+      <c r="J85" s="23"/>
+      <c r="K85" s="23"/>
+      <c r="L85" s="23"/>
+      <c r="M85" s="23"/>
+      <c r="N85" s="23"/>
+      <c r="O85" s="23"/>
+      <c r="P85" s="23"/>
+      <c r="Q85" s="23"/>
+      <c r="R85" s="23"/>
+      <c r="S85" s="23"/>
+      <c r="T85" s="23"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="23"/>
+      <c r="W85" s="23"/>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A86" s="27"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="27"/>
-      <c r="L86" s="27"/>
-      <c r="M86" s="27"/>
-      <c r="N86" s="27"/>
-      <c r="O86" s="27"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="27"/>
-      <c r="R86" s="27"/>
-      <c r="S86" s="27"/>
-      <c r="T86" s="27"/>
-      <c r="U86" s="27"/>
-      <c r="V86" s="27"/>
-      <c r="W86" s="27"/>
+      <c r="A86" s="23"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="23"/>
+      <c r="K86" s="23"/>
+      <c r="L86" s="23"/>
+      <c r="M86" s="23"/>
+      <c r="N86" s="23"/>
+      <c r="O86" s="23"/>
+      <c r="P86" s="23"/>
+      <c r="Q86" s="23"/>
+      <c r="R86" s="23"/>
+      <c r="S86" s="23"/>
+      <c r="T86" s="23"/>
+      <c r="U86" s="23"/>
+      <c r="V86" s="23"/>
+      <c r="W86" s="23"/>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A87" s="27"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="27"/>
-      <c r="K87" s="27"/>
-      <c r="L87" s="27"/>
-      <c r="M87" s="27"/>
-      <c r="N87" s="27"/>
-      <c r="O87" s="27"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="27"/>
-      <c r="R87" s="27"/>
-      <c r="S87" s="27"/>
-      <c r="T87" s="27"/>
-      <c r="U87" s="27"/>
-      <c r="V87" s="27"/>
-      <c r="W87" s="27"/>
+      <c r="A87" s="23"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="23"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="23"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="23"/>
+      <c r="N87" s="23"/>
+      <c r="O87" s="23"/>
+      <c r="P87" s="23"/>
+      <c r="Q87" s="23"/>
+      <c r="R87" s="23"/>
+      <c r="S87" s="23"/>
+      <c r="T87" s="23"/>
+      <c r="U87" s="23"/>
+      <c r="V87" s="23"/>
+      <c r="W87" s="23"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A88" s="27"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="27"/>
-      <c r="I88" s="27"/>
-      <c r="J88" s="27"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="27"/>
-      <c r="M88" s="27"/>
-      <c r="N88" s="27"/>
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="R88" s="27"/>
-      <c r="S88" s="27"/>
-      <c r="T88" s="27"/>
-      <c r="U88" s="27"/>
-      <c r="V88" s="27"/>
-      <c r="W88" s="27"/>
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="23"/>
+      <c r="K88" s="23"/>
+      <c r="L88" s="23"/>
+      <c r="M88" s="23"/>
+      <c r="N88" s="23"/>
+      <c r="O88" s="23"/>
+      <c r="P88" s="23"/>
+      <c r="Q88" s="23"/>
+      <c r="R88" s="23"/>
+      <c r="S88" s="23"/>
+      <c r="T88" s="23"/>
+      <c r="U88" s="23"/>
+      <c r="V88" s="23"/>
+      <c r="W88" s="23"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="27"/>
-      <c r="R89" s="27"/>
-      <c r="S89" s="27"/>
-      <c r="T89" s="27"/>
-      <c r="U89" s="27"/>
-      <c r="V89" s="27"/>
-      <c r="W89" s="27"/>
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="23"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="23"/>
+      <c r="P89" s="23"/>
+      <c r="Q89" s="23"/>
+      <c r="R89" s="23"/>
+      <c r="S89" s="23"/>
+      <c r="T89" s="23"/>
+      <c r="U89" s="23"/>
+      <c r="V89" s="23"/>
+      <c r="W89" s="23"/>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A90" s="27"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="27"/>
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
-      <c r="M90" s="27"/>
-      <c r="N90" s="27"/>
-      <c r="O90" s="27"/>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="27"/>
-      <c r="R90" s="27"/>
-      <c r="S90" s="27"/>
-      <c r="T90" s="27"/>
-      <c r="U90" s="27"/>
-      <c r="V90" s="27"/>
-      <c r="W90" s="27"/>
+      <c r="A90" s="23"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+      <c r="J90" s="23"/>
+      <c r="K90" s="23"/>
+      <c r="L90" s="23"/>
+      <c r="M90" s="23"/>
+      <c r="N90" s="23"/>
+      <c r="O90" s="23"/>
+      <c r="P90" s="23"/>
+      <c r="Q90" s="23"/>
+      <c r="R90" s="23"/>
+      <c r="S90" s="23"/>
+      <c r="T90" s="23"/>
+      <c r="U90" s="23"/>
+      <c r="V90" s="23"/>
+      <c r="W90" s="23"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A91" s="27"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
-      <c r="M91" s="27"/>
-      <c r="N91" s="27"/>
-      <c r="O91" s="27"/>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="27"/>
-      <c r="R91" s="27"/>
-      <c r="S91" s="27"/>
-      <c r="T91" s="27"/>
-      <c r="U91" s="27"/>
-      <c r="V91" s="27"/>
-      <c r="W91" s="27"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="23"/>
+      <c r="K91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="23"/>
+      <c r="N91" s="23"/>
+      <c r="O91" s="23"/>
+      <c r="P91" s="23"/>
+      <c r="Q91" s="23"/>
+      <c r="R91" s="23"/>
+      <c r="S91" s="23"/>
+      <c r="T91" s="23"/>
+      <c r="U91" s="23"/>
+      <c r="V91" s="23"/>
+      <c r="W91" s="23"/>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A92" s="27"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="N92" s="27"/>
-      <c r="O92" s="27"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="27"/>
-      <c r="R92" s="27"/>
-      <c r="S92" s="27"/>
-      <c r="T92" s="27"/>
-      <c r="U92" s="27"/>
-      <c r="V92" s="27"/>
-      <c r="W92" s="27"/>
+      <c r="A92" s="23"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
+      <c r="I92" s="23"/>
+      <c r="J92" s="23"/>
+      <c r="K92" s="23"/>
+      <c r="L92" s="23"/>
+      <c r="M92" s="23"/>
+      <c r="N92" s="23"/>
+      <c r="O92" s="23"/>
+      <c r="P92" s="23"/>
+      <c r="Q92" s="23"/>
+      <c r="R92" s="23"/>
+      <c r="S92" s="23"/>
+      <c r="T92" s="23"/>
+      <c r="U92" s="23"/>
+      <c r="V92" s="23"/>
+      <c r="W92" s="23"/>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A93" s="27"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="N93" s="27"/>
-      <c r="O93" s="27"/>
-      <c r="P93" s="27"/>
-      <c r="Q93" s="27"/>
-      <c r="R93" s="27"/>
-      <c r="S93" s="27"/>
-      <c r="T93" s="27"/>
-      <c r="U93" s="27"/>
-      <c r="V93" s="27"/>
-      <c r="W93" s="27"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="23"/>
+      <c r="I93" s="23"/>
+      <c r="J93" s="23"/>
+      <c r="K93" s="23"/>
+      <c r="L93" s="23"/>
+      <c r="M93" s="23"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
+      <c r="P93" s="23"/>
+      <c r="Q93" s="23"/>
+      <c r="R93" s="23"/>
+      <c r="S93" s="23"/>
+      <c r="T93" s="23"/>
+      <c r="U93" s="23"/>
+      <c r="V93" s="23"/>
+      <c r="W93" s="23"/>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A94" s="27"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
-      <c r="M94" s="27"/>
-      <c r="N94" s="27"/>
-      <c r="O94" s="27"/>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="27"/>
-      <c r="R94" s="27"/>
-      <c r="S94" s="27"/>
-      <c r="T94" s="27"/>
-      <c r="U94" s="27"/>
-      <c r="V94" s="27"/>
-      <c r="W94" s="27"/>
+      <c r="A94" s="23"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="23"/>
+      <c r="J94" s="23"/>
+      <c r="K94" s="23"/>
+      <c r="L94" s="23"/>
+      <c r="M94" s="23"/>
+      <c r="N94" s="23"/>
+      <c r="O94" s="23"/>
+      <c r="P94" s="23"/>
+      <c r="Q94" s="23"/>
+      <c r="R94" s="23"/>
+      <c r="S94" s="23"/>
+      <c r="T94" s="23"/>
+      <c r="U94" s="23"/>
+      <c r="V94" s="23"/>
+      <c r="W94" s="23"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A95" s="27"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
-      <c r="M95" s="27"/>
-      <c r="N95" s="27"/>
-      <c r="O95" s="27"/>
-      <c r="P95" s="27"/>
-      <c r="Q95" s="27"/>
-      <c r="R95" s="27"/>
-      <c r="S95" s="27"/>
-      <c r="T95" s="27"/>
-      <c r="U95" s="27"/>
-      <c r="V95" s="27"/>
-      <c r="W95" s="27"/>
+      <c r="A95" s="23"/>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="23"/>
+      <c r="J95" s="23"/>
+      <c r="K95" s="23"/>
+      <c r="L95" s="23"/>
+      <c r="M95" s="23"/>
+      <c r="N95" s="23"/>
+      <c r="O95" s="23"/>
+      <c r="P95" s="23"/>
+      <c r="Q95" s="23"/>
+      <c r="R95" s="23"/>
+      <c r="S95" s="23"/>
+      <c r="T95" s="23"/>
+      <c r="U95" s="23"/>
+      <c r="V95" s="23"/>
+      <c r="W95" s="23"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
-      <c r="M96" s="27"/>
-      <c r="N96" s="27"/>
-      <c r="O96" s="27"/>
-      <c r="P96" s="27"/>
-      <c r="Q96" s="27"/>
-      <c r="R96" s="27"/>
-      <c r="S96" s="27"/>
-      <c r="T96" s="27"/>
-      <c r="U96" s="27"/>
-      <c r="V96" s="27"/>
-      <c r="W96" s="27"/>
+      <c r="A96" s="23"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="23"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="23"/>
+      <c r="K96" s="23"/>
+      <c r="L96" s="23"/>
+      <c r="M96" s="23"/>
+      <c r="N96" s="23"/>
+      <c r="O96" s="23"/>
+      <c r="P96" s="23"/>
+      <c r="Q96" s="23"/>
+      <c r="R96" s="23"/>
+      <c r="S96" s="23"/>
+      <c r="T96" s="23"/>
+      <c r="U96" s="23"/>
+      <c r="V96" s="23"/>
+      <c r="W96" s="23"/>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A97" s="27"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
-      <c r="M97" s="27"/>
-      <c r="N97" s="27"/>
-      <c r="O97" s="27"/>
-      <c r="P97" s="27"/>
-      <c r="Q97" s="27"/>
-      <c r="R97" s="27"/>
-      <c r="S97" s="27"/>
-      <c r="T97" s="27"/>
-      <c r="U97" s="27"/>
-      <c r="V97" s="27"/>
-      <c r="W97" s="27"/>
+      <c r="A97" s="23"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23"/>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
+      <c r="K97" s="23"/>
+      <c r="L97" s="23"/>
+      <c r="M97" s="23"/>
+      <c r="N97" s="23"/>
+      <c r="O97" s="23"/>
+      <c r="P97" s="23"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="23"/>
+      <c r="S97" s="23"/>
+      <c r="T97" s="23"/>
+      <c r="U97" s="23"/>
+      <c r="V97" s="23"/>
+      <c r="W97" s="23"/>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A98" s="27"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-      <c r="O98" s="27"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="27"/>
-      <c r="R98" s="27"/>
-      <c r="S98" s="27"/>
-      <c r="T98" s="27"/>
-      <c r="U98" s="27"/>
-      <c r="V98" s="27"/>
-      <c r="W98" s="27"/>
+      <c r="A98" s="23"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="23"/>
+      <c r="I98" s="23"/>
+      <c r="J98" s="23"/>
+      <c r="K98" s="23"/>
+      <c r="L98" s="23"/>
+      <c r="M98" s="23"/>
+      <c r="N98" s="23"/>
+      <c r="O98" s="23"/>
+      <c r="P98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="23"/>
+      <c r="S98" s="23"/>
+      <c r="T98" s="23"/>
+      <c r="U98" s="23"/>
+      <c r="V98" s="23"/>
+      <c r="W98" s="23"/>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
-      <c r="M99" s="27"/>
-      <c r="N99" s="27"/>
-      <c r="O99" s="27"/>
-      <c r="P99" s="27"/>
-      <c r="Q99" s="27"/>
-      <c r="R99" s="27"/>
-      <c r="S99" s="27"/>
-      <c r="T99" s="27"/>
-      <c r="U99" s="27"/>
-      <c r="V99" s="27"/>
-      <c r="W99" s="27"/>
+      <c r="A99" s="23"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="23"/>
+      <c r="I99" s="23"/>
+      <c r="J99" s="23"/>
+      <c r="K99" s="23"/>
+      <c r="L99" s="23"/>
+      <c r="M99" s="23"/>
+      <c r="N99" s="23"/>
+      <c r="O99" s="23"/>
+      <c r="P99" s="23"/>
+      <c r="Q99" s="23"/>
+      <c r="R99" s="23"/>
+      <c r="S99" s="23"/>
+      <c r="T99" s="23"/>
+      <c r="U99" s="23"/>
+      <c r="V99" s="23"/>
+      <c r="W99" s="23"/>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
-      <c r="M100" s="27"/>
-      <c r="N100" s="27"/>
-      <c r="O100" s="27"/>
-      <c r="P100" s="27"/>
-      <c r="Q100" s="27"/>
-      <c r="R100" s="27"/>
-      <c r="S100" s="27"/>
-      <c r="T100" s="27"/>
-      <c r="U100" s="27"/>
-      <c r="V100" s="27"/>
-      <c r="W100" s="27"/>
+      <c r="K100" s="23"/>
+      <c r="L100" s="23"/>
+      <c r="M100" s="23"/>
+      <c r="N100" s="23"/>
+      <c r="O100" s="23"/>
+      <c r="P100" s="23"/>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="23"/>
+      <c r="S100" s="23"/>
+      <c r="T100" s="23"/>
+      <c r="U100" s="23"/>
+      <c r="V100" s="23"/>
+      <c r="W100" s="23"/>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
-      <c r="M101" s="27"/>
-      <c r="N101" s="27"/>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="27"/>
-      <c r="R101" s="27"/>
-      <c r="S101" s="27"/>
-      <c r="T101" s="27"/>
-      <c r="U101" s="27"/>
-      <c r="V101" s="27"/>
-      <c r="W101" s="27"/>
+      <c r="K101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="M101" s="23"/>
+      <c r="N101" s="23"/>
+      <c r="O101" s="23"/>
+      <c r="P101" s="23"/>
+      <c r="Q101" s="23"/>
+      <c r="R101" s="23"/>
+      <c r="S101" s="23"/>
+      <c r="T101" s="23"/>
+      <c r="U101" s="23"/>
+      <c r="V101" s="23"/>
+      <c r="W101" s="23"/>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K102" s="23"/>
+      <c r="L102" s="23"/>
+      <c r="M102" s="23"/>
+      <c r="N102" s="23"/>
+      <c r="O102" s="23"/>
+      <c r="P102" s="23"/>
+      <c r="Q102" s="23"/>
+      <c r="R102" s="23"/>
+      <c r="S102" s="23"/>
+      <c r="T102" s="23"/>
+      <c r="U102" s="23"/>
+      <c r="V102" s="23"/>
+      <c r="W102" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>